<commit_message>
Wrote a very basic script for generating a battery pack based on minimum voltage and current
</commit_message>
<xml_diff>
--- a/PowertrainV2/Powertrain Simulation Data.xlsx
+++ b/PowertrainV2/Powertrain Simulation Data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://virginiatech-my.sharepoint.com/personal/kdubbbz_vt_edu/Documents/Documents/BOLT/BOLT projects/Powertrain Simulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trevl\Desktop\Projects\PowertrainSimulation\PowertrainV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{176D5D3E-F989-4244-BC13-AD651FD3AAA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1ABB2A-276A-4998-9E20-C8F570C62797}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7635" yWindow="8355" windowWidth="21600" windowHeight="11835" xr2:uid="{8E9DA397-A3DF-49D6-A417-433341F270C1}"/>
+    <workbookView xWindow="1830" yWindow="4830" windowWidth="25680" windowHeight="14010" xr2:uid="{8E9DA397-A3DF-49D6-A417-433341F270C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Motors" sheetId="1" r:id="rId1"/>
     <sheet name="Motor_Controllers" sheetId="2" r:id="rId2"/>
-    <sheet name="Battery_Packs" sheetId="3" r:id="rId3"/>
+    <sheet name="Batteries" sheetId="5" r:id="rId3"/>
+    <sheet name="Battery_Packs" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Motors</t>
   </si>
@@ -149,13 +150,46 @@
   </si>
   <si>
     <t>Rinehart PM150DZR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery </t>
+  </si>
+  <si>
+    <t>Cell Weight (g)</t>
+  </si>
+  <si>
+    <t>Nominal Voltage</t>
+  </si>
+  <si>
+    <r>
+      <t>Max Internal Resistance (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω)</t>
+    </r>
+  </si>
+  <si>
+    <t>Nominal Capacity (Ah)</t>
+  </si>
+  <si>
+    <t>LIR 18650</t>
+  </si>
+  <si>
+    <t>Cost Per Cell (USD)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +219,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -601,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -612,85 +653,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1010,7 +1060,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,60 +1071,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="6">
         <f>COUNTA(A3:B31)</f>
         <v>7</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="11">
+      <c r="B3" s="29"/>
+      <c r="C3" s="7">
         <v>10</v>
       </c>
       <c r="D3" s="2">
@@ -1092,10 +1142,10 @@
       <c r="H3" s="2">
         <v>9000</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I3" s="20">
         <v>4</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="11">
         <v>0.01</v>
       </c>
     </row>
@@ -1104,7 +1154,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="24"/>
-      <c r="C4" s="12">
+      <c r="C4" s="8">
         <v>20</v>
       </c>
       <c r="D4" s="3">
@@ -1122,10 +1172,10 @@
       <c r="H4" s="3">
         <v>8000</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="21">
         <v>4</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="12">
         <v>0.02</v>
       </c>
     </row>
@@ -1134,7 +1184,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="24"/>
-      <c r="C5" s="12">
+      <c r="C5" s="8">
         <v>14</v>
       </c>
       <c r="D5" s="3">
@@ -1152,10 +1202,10 @@
       <c r="H5" s="3">
         <v>10000</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="21">
         <v>4</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="12">
         <v>0.03</v>
       </c>
     </row>
@@ -1164,7 +1214,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="24"/>
-      <c r="C6" s="12">
+      <c r="C6" s="8">
         <v>16</v>
       </c>
       <c r="D6" s="3">
@@ -1182,10 +1232,10 @@
       <c r="H6" s="3">
         <v>12000</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="21">
         <v>4</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="12">
         <v>0.04</v>
       </c>
     </row>
@@ -1194,7 +1244,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="24"/>
-      <c r="C7" s="12"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3">
@@ -1202,17 +1252,17 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="29">
+      <c r="I7" s="21">
         <v>4</v>
       </c>
-      <c r="J7" s="16"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="24"/>
-      <c r="C8" s="12">
+      <c r="C8" s="8">
         <v>115</v>
       </c>
       <c r="D8" s="3">
@@ -1230,17 +1280,17 @@
       <c r="H8" s="3">
         <v>12000</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="21">
         <v>3.5</v>
       </c>
-      <c r="J8" s="16"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="24"/>
-      <c r="C9" s="12">
+      <c r="C9" s="8">
         <v>250</v>
       </c>
       <c r="D9" s="3">
@@ -1258,22 +1308,22 @@
       <c r="H9" s="3">
         <v>8000</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I9" s="21">
         <v>0.34693878</v>
       </c>
-      <c r="J9" s="16"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="18"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1309,134 +1359,277 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="8"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="6">
         <f>COUNTA(A3:B31)</f>
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="11">
+      <c r="B3" s="32"/>
+      <c r="C3" s="7">
         <v>10</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="11">
         <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="12">
+      <c r="B4" s="32"/>
+      <c r="C4" s="8">
         <v>20</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="12">
         <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="12">
+      <c r="B5" s="32"/>
+      <c r="C5" s="8">
         <v>14</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="12">
         <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="12">
+      <c r="B6" s="32"/>
+      <c r="C6" s="8">
         <v>16</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="12">
         <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="12">
+      <c r="B7" s="32"/>
+      <c r="C7" s="8">
         <v>7.5</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="12">
+      <c r="B8" s="32"/>
+      <c r="C8" s="8">
         <v>10.7</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="16"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CEB787-78C8-4127-AE45-B4F69E1F9640}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="10" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7">
+        <v>3.7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>46.5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC148048-313D-4336-880C-48A7AE95656F}">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,60 +1640,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="6">
         <f>COUNTA(A3:B31)</f>
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="11">
+      <c r="B3" s="29"/>
+      <c r="C3" s="7">
         <v>4.2</v>
       </c>
       <c r="D3" s="2">
@@ -1515,15 +1708,15 @@
       <c r="G3" s="2">
         <v>0.05</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="20">
         <f>E3*C3</f>
         <v>25.200000000000003</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I3" s="20">
         <f>D3*F3</f>
         <v>431.6</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="11">
         <f>H3*I3</f>
         <v>10876.320000000002</v>
       </c>
@@ -1533,7 +1726,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="24"/>
-      <c r="C4" s="12">
+      <c r="C4" s="8">
         <v>4.2</v>
       </c>
       <c r="D4" s="3">
@@ -1548,15 +1741,15 @@
       <c r="G4" s="3">
         <v>0.02</v>
       </c>
-      <c r="H4" s="29">
+      <c r="H4" s="21">
         <f t="shared" ref="H4:H5" si="0">E4*C4</f>
         <v>16.8</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="21">
         <f t="shared" ref="I4:I5" si="1">D4*F4</f>
         <v>585</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="12">
         <f t="shared" ref="J4:J5" si="2">H4*I4</f>
         <v>9828</v>
       </c>
@@ -1566,7 +1759,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="24"/>
-      <c r="C5" s="12">
+      <c r="C5" s="8">
         <v>4.2</v>
       </c>
       <c r="D5" s="3">
@@ -1581,15 +1774,15 @@
       <c r="G5" s="3">
         <v>0.06</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="21">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="21">
         <f t="shared" si="1"/>
         <v>260</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="12">
         <f t="shared" si="2"/>
         <v>10920</v>
       </c>
@@ -1599,7 +1792,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="24"/>
-      <c r="C6" s="12">
+      <c r="C6" s="8">
         <v>3.7</v>
       </c>
       <c r="D6" s="3">
@@ -1608,21 +1801,21 @@
       <c r="E6" s="3">
         <v>78</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="21">
         <v>4</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="21">
         <v>0.01</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="21">
         <f t="shared" ref="H6:H7" si="3">E6*C6</f>
         <v>288.60000000000002</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="21">
         <f t="shared" ref="I6:I7" si="4">D6*F6</f>
         <v>40</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="12">
         <f t="shared" ref="J6:J7" si="5">H6*I6</f>
         <v>11544</v>
       </c>
@@ -1632,7 +1825,7 @@
         <v>31</v>
       </c>
       <c r="B7" s="24"/>
-      <c r="C7" s="12">
+      <c r="C7" s="8">
         <v>3.6</v>
       </c>
       <c r="D7" s="3">
@@ -1641,21 +1834,21 @@
       <c r="E7" s="3">
         <v>166</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="21">
         <v>6</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="21">
         <v>0.01</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="21">
         <f t="shared" si="3"/>
         <v>597.6</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="21">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="12">
         <f t="shared" si="5"/>
         <v>10756.800000000001</v>
       </c>
@@ -1663,58 +1856,73 @@
     <row r="8" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23"/>
       <c r="B8" s="24"/>
-      <c r="C8" s="12"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="16"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24"/>
-      <c r="C9" s="12"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="16"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="18"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7DE497FA346CD49B765B54AB6A367B5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a083ce2df5f3fd6d0cb1a91bb80a39cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d9c5c803-e33e-4c61-8351-da4c9b99ae39" xmlns:ns4="6be6f6fe-38a0-487d-a8a9-15e966a8f4d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a231930d9aebb724d1ef5c3843d36139" ns3:_="" ns4:_="">
     <xsd:import namespace="d9c5c803-e33e-4c61-8351-da4c9b99ae39"/>
@@ -1931,22 +2139,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C91FC5E-A7AE-47CB-B37A-F40974CEFF68}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2CC42D-DFF7-4C9F-AB84-7709A2108688}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3AAEA67-50ED-417A-8971-4D32193B67A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1963,21 +2173,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2CC42D-DFF7-4C9F-AB84-7709A2108688}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C91FC5E-A7AE-47CB-B37A-F40974CEFF68}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Script can now generate all possible configurations in a range of voltage and current. Now writes to a CSV.
</commit_message>
<xml_diff>
--- a/PowertrainV2/Powertrain Simulation Data.xlsx
+++ b/PowertrainV2/Powertrain Simulation Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trevl\Desktop\Projects\PowertrainSimulation\PowertrainV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1ABB2A-276A-4998-9E20-C8F570C62797}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979F546D-4FDA-46C1-ABA2-A89AF8E420FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="4830" windowWidth="25680" windowHeight="14010" xr2:uid="{8E9DA397-A3DF-49D6-A417-433341F270C1}"/>
+    <workbookView xWindow="1830" yWindow="4830" windowWidth="25680" windowHeight="14010" activeTab="2" xr2:uid="{8E9DA397-A3DF-49D6-A417-433341F270C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Motors" sheetId="1" r:id="rId1"/>
@@ -1059,7 +1059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CE18CD-D822-4FAB-A7CC-DC557D973563}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -1466,16 +1466,16 @@
     <row r="11" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1485,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CEB787-78C8-4127-AE45-B4F69E1F9640}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,16 +1892,16 @@
     <row r="11" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1914,15 +1914,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7DE497FA346CD49B765B54AB6A367B5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a083ce2df5f3fd6d0cb1a91bb80a39cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d9c5c803-e33e-4c61-8351-da4c9b99ae39" xmlns:ns4="6be6f6fe-38a0-487d-a8a9-15e966a8f4d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a231930d9aebb724d1ef5c3843d36139" ns3:_="" ns4:_="">
     <xsd:import namespace="d9c5c803-e33e-4c61-8351-da4c9b99ae39"/>
@@ -2139,6 +2130,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C91FC5E-A7AE-47CB-B37A-F40974CEFF68}">
   <ds:schemaRefs>
@@ -2149,14 +2149,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2CC42D-DFF7-4C9F-AB84-7709A2108688}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3AAEA67-50ED-417A-8971-4D32193B67A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2173,4 +2165,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2CC42D-DFF7-4C9F-AB84-7709A2108688}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Script now generates pack configurations based off of motor controller specs
</commit_message>
<xml_diff>
--- a/PowertrainV2/Powertrain Simulation Data.xlsx
+++ b/PowertrainV2/Powertrain Simulation Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trevl\Desktop\Projects\PowertrainSimulation\PowertrainV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979F546D-4FDA-46C1-ABA2-A89AF8E420FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD6BF9B-BDE4-412F-A0BC-587FD33E92F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="4830" windowWidth="25680" windowHeight="14010" activeTab="2" xr2:uid="{8E9DA397-A3DF-49D6-A417-433341F270C1}"/>
+    <workbookView xWindow="24090" yWindow="5250" windowWidth="25680" windowHeight="14010" activeTab="1" xr2:uid="{8E9DA397-A3DF-49D6-A417-433341F270C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Motors" sheetId="1" r:id="rId1"/>
-    <sheet name="Motor_Controllers" sheetId="2" r:id="rId2"/>
+    <sheet name="MotorControllers" sheetId="6" r:id="rId2"/>
     <sheet name="Batteries" sheetId="5" r:id="rId3"/>
     <sheet name="Battery_Packs" sheetId="3" r:id="rId4"/>
+    <sheet name="Motor_Controllers" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Motors</t>
   </si>
@@ -183,6 +184,27 @@
   </si>
   <si>
     <t>Cost Per Cell (USD)</t>
+  </si>
+  <si>
+    <t>Motor Controller</t>
+  </si>
+  <si>
+    <t>Max Op Voltage (V)</t>
+  </si>
+  <si>
+    <t>Max NonOp Voltage (V)</t>
+  </si>
+  <si>
+    <t>Current Continuous (Arms)</t>
+  </si>
+  <si>
+    <t>Current Peak (Arms)</t>
+  </si>
+  <si>
+    <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>Rinehart PM150DZ</t>
   </si>
 </sst>
 </file>
@@ -642,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -708,6 +730,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1060,7 +1085,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,20 +1096,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1120,10 +1145,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="7">
         <v>10</v>
       </c>
@@ -1150,10 +1175,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="8">
         <v>20</v>
       </c>
@@ -1180,10 +1205,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="8">
         <v>14</v>
       </c>
@@ -1210,10 +1235,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="8">
         <v>16</v>
       </c>
@@ -1240,10 +1265,10 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="8"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1258,10 +1283,10 @@
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="8">
         <v>115</v>
       </c>
@@ -1286,10 +1311,10 @@
       <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="24"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="8">
         <v>250</v>
       </c>
@@ -1314,8 +1339,8 @@
       <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="13"/>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
@@ -1345,138 +1370,108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79F4363-D78F-4A86-A11E-F562969018DF}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0AD601F-A724-4372-B860-9EDCE8EEBEBE}">
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="27"/>
-    </row>
-    <row r="2" spans="1:4" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="6">
-        <f>COUNTA(A3:B31)</f>
-        <v>6</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="7">
-        <v>10</v>
-      </c>
-      <c r="D3" s="11">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="8">
-        <v>20</v>
-      </c>
-      <c r="D4" s="12">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="8">
-        <v>14</v>
-      </c>
-      <c r="D5" s="12">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="8">
-        <v>16</v>
-      </c>
-      <c r="D6" s="12">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
+    <row r="1" spans="1:6" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="8">
+      <c r="B2" s="7">
+        <v>400</v>
+      </c>
+      <c r="C2" s="2">
+        <v>500</v>
+      </c>
+      <c r="D2" s="2">
+        <v>300</v>
+      </c>
+      <c r="E2" s="2">
+        <v>450</v>
+      </c>
+      <c r="F2" s="2">
         <v>7.5</v>
       </c>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="8">
+    </row>
+    <row r="3" spans="1:6" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="7">
+        <v>720</v>
+      </c>
+      <c r="C3" s="2">
+        <v>900</v>
+      </c>
+      <c r="D3" s="2">
+        <v>225</v>
+      </c>
+      <c r="E3" s="2">
+        <v>300</v>
+      </c>
+      <c r="F3" s="2">
         <v>10.7</v>
       </c>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="33"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="4" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+    </row>
+    <row r="6" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+    </row>
+    <row r="9" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1485,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CEB787-78C8-4127-AE45-B4F69E1F9640}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,20 +1635,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1689,10 +1684,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="7">
         <v>4.2</v>
       </c>
@@ -1722,10 +1717,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="8">
         <v>4.2</v>
       </c>
@@ -1755,10 +1750,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="8">
         <v>4.2</v>
       </c>
@@ -1788,10 +1783,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="8">
         <v>3.7</v>
       </c>
@@ -1821,10 +1816,10 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="8">
         <v>3.6</v>
       </c>
@@ -1854,8 +1849,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="8"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1866,8 +1861,8 @@
       <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="8"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1878,8 +1873,8 @@
       <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="13"/>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
@@ -1892,16 +1887,153 @@
     <row r="11" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79F4363-D78F-4A86-A11E-F562969018DF}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6">
+        <f>COUNTA(A3:B31)</f>
+        <v>6</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="7">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="8">
+        <v>20</v>
+      </c>
+      <c r="D4" s="12">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="8">
+        <v>14</v>
+      </c>
+      <c r="D5" s="12">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="8">
+        <v>16</v>
+      </c>
+      <c r="D6" s="12">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="8">
+        <v>10.7</v>
+      </c>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="34"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C1:D1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1914,6 +2046,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7DE497FA346CD49B765B54AB6A367B5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a083ce2df5f3fd6d0cb1a91bb80a39cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d9c5c803-e33e-4c61-8351-da4c9b99ae39" xmlns:ns4="6be6f6fe-38a0-487d-a8a9-15e966a8f4d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a231930d9aebb724d1ef5c3843d36139" ns3:_="" ns4:_="">
     <xsd:import namespace="d9c5c803-e33e-4c61-8351-da4c9b99ae39"/>
@@ -2130,15 +2271,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C91FC5E-A7AE-47CB-B37A-F40974CEFF68}">
   <ds:schemaRefs>
@@ -2149,6 +2281,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2CC42D-DFF7-4C9F-AB84-7709A2108688}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3AAEA67-50ED-417A-8971-4D32193B67A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2165,12 +2305,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2CC42D-DFF7-4C9F-AB84-7709A2108688}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>